<commit_message>
separated crawler2 into files
</commit_message>
<xml_diff>
--- a/cookie_data.xlsx
+++ b/cookie_data.xlsx
@@ -503,7 +503,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-09-02 17:34:31</t>
+          <t>2024-09-02 18:07:55</t>
         </is>
       </c>
       <c r="D2" t="b">
@@ -541,7 +541,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>23h 59m 44s</t>
+          <t>23h 59m 42s</t>
         </is>
       </c>
     </row>
@@ -558,7 +558,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2024-09-02 17:34:31</t>
+          <t>2024-09-02 18:07:55</t>
         </is>
       </c>
       <c r="D3" t="b">
@@ -596,7 +596,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>23h 59m 39s</t>
+          <t>23h 59m 37s</t>
         </is>
       </c>
     </row>
@@ -613,7 +613,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2023-09-10 17:35:00</t>
+          <t>2023-09-10 18:08:25</t>
         </is>
       </c>
       <c r="D4" t="b">
@@ -668,7 +668,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2023-09-04 17:35:00</t>
+          <t>2023-09-04 18:08:25</t>
         </is>
       </c>
       <c r="D5" t="b">
@@ -723,7 +723,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2024-10-07 17:35:00</t>
+          <t>2024-10-07 18:08:25</t>
         </is>
       </c>
       <c r="D6" t="b">
@@ -778,7 +778,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2023-09-10 17:35:00</t>
+          <t>2023-09-10 18:08:25</t>
         </is>
       </c>
       <c r="D7" t="b">

</xml_diff>

<commit_message>
sperated crawler into componenents
</commit_message>
<xml_diff>
--- a/cookie_data.xlsx
+++ b/cookie_data.xlsx
@@ -425,26 +425,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="27" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="21" customWidth="1" min="3" max="3"/>
-    <col width="8" customWidth="1" min="4" max="4"/>
-    <col width="16" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="10" customWidth="1" min="7" max="7"/>
-    <col width="14" customWidth="1" min="8" max="8"/>
-    <col width="24" customWidth="1" min="9" max="9"/>
-    <col width="19" customWidth="1" min="10" max="10"/>
-    <col width="13" customWidth="1" min="11" max="11"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -516,7 +503,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-09-02 23:26:19</t>
+          <t>2024-09-03 14:24:16</t>
         </is>
       </c>
       <c r="D2" t="b">
@@ -554,7 +541,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>23h 59m 44s</t>
+          <t>23h 59m 43s</t>
         </is>
       </c>
     </row>
@@ -571,7 +558,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2024-09-02 23:26:19</t>
+          <t>2024-09-03 14:24:16</t>
         </is>
       </c>
       <c r="D3" t="b">
@@ -608,6 +595,116 @@
         </is>
       </c>
       <c r="K3" t="inlineStr">
+        <is>
+          <t>23h 59m 38s</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>osano_consentmanager</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>.victorinsurance.nl</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2024-09-03 14:24:48</t>
+        </is>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Osano</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Type1 (Manage Cookies)</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>23h 59m 44s</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>osano_consentmanager_uuid</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>.victorinsurance.nl</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2024-09-03 14:24:48</t>
+        </is>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Osano</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Type1 (Manage Cookies)</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
         <is>
           <t>23h 59m 39s</t>
         </is>

</xml_diff>

<commit_message>
fixed manage cookies link in other languages
</commit_message>
<xml_diff>
--- a/cookie_data.xlsx
+++ b/cookie_data.xlsx
@@ -498,12 +498,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>.ironwoodins.com</t>
+          <t>.victorinsurance.nl</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-09-04 17:51:56</t>
+          <t>2024-09-05 22:12:04</t>
         </is>
       </c>
       <c r="D2" t="b">
@@ -553,12 +553,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>.ironwoodins.com</t>
+          <t>.victorinsurance.nl</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2024-09-04 17:51:56</t>
+          <t>2024-09-05 22:12:04</t>
         </is>
       </c>
       <c r="D3" t="b">

</xml_diff>